<commit_message>
INTERACTIVE MAP 0.1.1 toggle visibility on filters
</commit_message>
<xml_diff>
--- a/src/assets/data/agua_potable_producida/agua_potable_producida.xlsx
+++ b/src/assets/data/agua_potable_producida/agua_potable_producida.xlsx
@@ -16,7 +16,7 @@
     <t>Fecha</t>
   </si>
   <si>
-    <t>AP_Sup_Maipo</t>
+    <t>AP_Maipo</t>
   </si>
   <si>
     <t>AP_Sup_01</t>
@@ -1189,7 +1189,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>

</xml_diff>